<commit_message>
add excel about commit
</commit_message>
<xml_diff>
--- a/team103项目总结报告/开发和测试过程数据统计对照表103.xlsx
+++ b/team103项目总结报告/开发和测试过程数据统计对照表103.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cqx\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Team103\team103项目总结报告\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D1C800-5750-4D81-885C-C895585F7264}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9750" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="对照表" sheetId="1" r:id="rId1"/>
@@ -18,18 +19,11 @@
     <sheet name="测试统计表" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="281">
   <si>
     <t>Github账户</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -658,9 +652,6 @@
   </si>
   <si>
     <t>测试通过网页显示机器人状态</t>
-  </si>
-  <si>
-    <t>KL-C-U-1</t>
   </si>
   <si>
     <t>测试通过网页按键点击，停止机器人运动</t>
@@ -1091,11 +1082,35 @@
     <t>KL-C-X-X</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>周尚纯</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>55827ad</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加了急停恢复代码，改进了线程阻塞与安全相关设置</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>4b0b63d</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加了急停、恢复的服务器端代码，在脚本客户端增加收消息功能</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>KL-C-U-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
@@ -1736,33 +1751,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P228"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.58203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.25" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.58203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="11" style="1" customWidth="1"/>
     <col min="12" max="12" width="10.5" style="1" customWidth="1"/>
     <col min="13" max="13" width="11.25" style="1" customWidth="1"/>
-    <col min="14" max="16" width="12.875" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.625" style="1"/>
+    <col min="14" max="16" width="12.83203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.58203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" ht="21.5" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>16</v>
       </c>
@@ -1772,13 +1787,13 @@
       <c r="E1" s="35"/>
       <c r="F1" s="35"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
@@ -1788,13 +1803,13 @@
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="B5" s="10" t="s">
         <v>2</v>
@@ -1812,7 +1827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>0</v>
       </c>
@@ -1832,7 +1847,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>1</v>
       </c>
@@ -1852,13 +1867,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
@@ -1872,7 +1887,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>1</v>
       </c>
@@ -1896,7 +1911,7 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>2</v>
       </c>
@@ -1920,7 +1935,7 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>3</v>
       </c>
@@ -1944,7 +1959,7 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>4</v>
       </c>
@@ -1952,10 +1967,10 @@
         <v>78</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="D13" s="22" t="s">
         <v>261</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>262</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1970,7 +1985,7 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>5</v>
       </c>
@@ -1978,10 +1993,10 @@
         <v>81</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D14" s="22" t="s">
         <v>263</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>264</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1996,7 +2011,7 @@
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
     </row>
-    <row r="15" spans="1:16" ht="70.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:16" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>6</v>
       </c>
@@ -2007,7 +2022,7 @@
         <v>117</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -2022,7 +2037,7 @@
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
     </row>
-    <row r="16" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>7</v>
       </c>
@@ -2044,7 +2059,7 @@
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
     </row>
-    <row r="17" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="12">
         <v>8</v>
       </c>
@@ -2055,7 +2070,7 @@
         <v>4662817</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -2070,7 +2085,7 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="12">
         <v>9</v>
       </c>
@@ -2078,10 +2093,10 @@
         <v>91</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -2094,7 +2109,7 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
     </row>
-    <row r="19" spans="1:16" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:16" ht="21.5" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
         <v>10</v>
       </c>
@@ -2102,10 +2117,10 @@
         <v>94</v>
       </c>
       <c r="C19" s="10" t="s">
+        <v>267</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>268</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>269</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
@@ -2120,7 +2135,7 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="12">
         <v>11</v>
       </c>
@@ -2128,10 +2143,10 @@
         <v>97</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -2144,7 +2159,7 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="12">
         <v>12</v>
       </c>
@@ -2152,10 +2167,10 @@
         <v>100</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
@@ -2168,7 +2183,7 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
         <v>13</v>
       </c>
@@ -2176,7 +2191,7 @@
         <v>102</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D22" s="10"/>
       <c r="G22" s="2"/>
@@ -2190,7 +2205,7 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="12">
         <v>14</v>
       </c>
@@ -2198,7 +2213,7 @@
         <v>104</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D23" s="10"/>
       <c r="G23" s="2"/>
@@ -2212,7 +2227,7 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
         <v>15</v>
       </c>
@@ -2223,7 +2238,7 @@
         <v>156</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -2236,7 +2251,7 @@
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
     </row>
-    <row r="25" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
         <v>16</v>
       </c>
@@ -2244,10 +2259,10 @@
         <v>108</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -2260,7 +2275,7 @@
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
         <v>17</v>
       </c>
@@ -2271,7 +2286,7 @@
         <v>126</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -2286,7 +2301,7 @@
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <v>18</v>
       </c>
@@ -2294,7 +2309,7 @@
         <v>113</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="2"/>
@@ -2310,7 +2325,7 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="12">
         <v>19</v>
       </c>
@@ -2332,7 +2347,7 @@
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
     </row>
-    <row r="29" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="7"/>
@@ -2350,7 +2365,7 @@
       <c r="O29" s="2"/>
       <c r="P29" s="2"/>
     </row>
-    <row r="30" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="7"/>
@@ -2368,7 +2383,7 @@
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
     </row>
-    <row r="31" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -2382,7 +2397,7 @@
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
     </row>
-    <row r="32" spans="1:16" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:16" ht="21.5" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>28</v>
       </c>
@@ -2402,7 +2417,7 @@
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
     </row>
-    <row r="33" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="14"/>
       <c r="B33" s="10" t="s">
         <v>2</v>
@@ -2430,7 +2445,7 @@
       <c r="O33" s="2"/>
       <c r="P33" s="2"/>
     </row>
-    <row r="34" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>1</v>
       </c>
@@ -2460,7 +2475,7 @@
       <c r="O34" s="2"/>
       <c r="P34" s="2"/>
     </row>
-    <row r="35" spans="1:16" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>29</v>
       </c>
@@ -2480,7 +2495,7 @@
       <c r="O35" s="2"/>
       <c r="P35" s="2"/>
     </row>
-    <row r="36" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="7"/>
@@ -2498,7 +2513,7 @@
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
     </row>
-    <row r="37" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>30</v>
       </c>
@@ -2520,7 +2535,7 @@
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
     </row>
-    <row r="38" spans="1:16" ht="51.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:16" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>31</v>
       </c>
@@ -2542,7 +2557,7 @@
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
     </row>
-    <row r="39" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2560,7 +2575,7 @@
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
     </row>
-    <row r="40" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2578,7 +2593,7 @@
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
     </row>
-    <row r="41" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2596,7 +2611,7 @@
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
     </row>
-    <row r="42" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2614,7 +2629,7 @@
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
     </row>
-    <row r="43" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2632,7 +2647,7 @@
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
     </row>
-    <row r="44" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2650,7 +2665,7 @@
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
     </row>
-    <row r="45" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2668,7 +2683,7 @@
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
     </row>
-    <row r="46" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2686,7 +2701,7 @@
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
     </row>
-    <row r="47" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2704,7 +2719,7 @@
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
     </row>
-    <row r="48" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2722,7 +2737,7 @@
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
     </row>
-    <row r="49" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2740,7 +2755,7 @@
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
     </row>
-    <row r="50" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2758,7 +2773,7 @@
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
     </row>
-    <row r="51" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2776,7 +2791,7 @@
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
     </row>
-    <row r="52" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2794,7 +2809,7 @@
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
     </row>
-    <row r="53" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2812,7 +2827,7 @@
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
     </row>
-    <row r="54" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2830,7 +2845,7 @@
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
     </row>
-    <row r="55" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2848,7 +2863,7 @@
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
     </row>
-    <row r="56" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2866,7 +2881,7 @@
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
     </row>
-    <row r="57" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2884,7 +2899,7 @@
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
     </row>
-    <row r="58" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2902,7 +2917,7 @@
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
     </row>
-    <row r="59" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2920,7 +2935,7 @@
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
     </row>
-    <row r="60" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2938,7 +2953,7 @@
       <c r="O60" s="2"/>
       <c r="P60" s="2"/>
     </row>
-    <row r="61" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2956,7 +2971,7 @@
       <c r="O61" s="2"/>
       <c r="P61" s="2"/>
     </row>
-    <row r="62" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2974,7 +2989,7 @@
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
     </row>
-    <row r="63" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2992,7 +3007,7 @@
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
     </row>
-    <row r="64" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -3010,7 +3025,7 @@
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
     </row>
-    <row r="65" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -3028,7 +3043,7 @@
       <c r="O65" s="2"/>
       <c r="P65" s="2"/>
     </row>
-    <row r="66" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -3046,7 +3061,7 @@
       <c r="O66" s="2"/>
       <c r="P66" s="2"/>
     </row>
-    <row r="67" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -3064,7 +3079,7 @@
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
     </row>
-    <row r="68" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -3082,7 +3097,7 @@
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
     </row>
-    <row r="69" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -3100,7 +3115,7 @@
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
     </row>
-    <row r="70" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -3118,7 +3133,7 @@
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
     </row>
-    <row r="71" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -3136,7 +3151,7 @@
       <c r="O71" s="2"/>
       <c r="P71" s="2"/>
     </row>
-    <row r="72" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -3154,7 +3169,7 @@
       <c r="O72" s="2"/>
       <c r="P72" s="2"/>
     </row>
-    <row r="73" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -3172,7 +3187,7 @@
       <c r="O73" s="2"/>
       <c r="P73" s="2"/>
     </row>
-    <row r="74" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -3190,7 +3205,7 @@
       <c r="O74" s="2"/>
       <c r="P74" s="2"/>
     </row>
-    <row r="75" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -3208,7 +3223,7 @@
       <c r="O75" s="2"/>
       <c r="P75" s="2"/>
     </row>
-    <row r="76" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -3226,7 +3241,7 @@
       <c r="O76" s="2"/>
       <c r="P76" s="2"/>
     </row>
-    <row r="77" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -3244,7 +3259,7 @@
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
     </row>
-    <row r="78" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -3262,7 +3277,7 @@
       <c r="O78" s="2"/>
       <c r="P78" s="2"/>
     </row>
-    <row r="79" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -3280,7 +3295,7 @@
       <c r="O79" s="2"/>
       <c r="P79" s="2"/>
     </row>
-    <row r="80" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -3298,7 +3313,7 @@
       <c r="O80" s="2"/>
       <c r="P80" s="2"/>
     </row>
-    <row r="81" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -3316,7 +3331,7 @@
       <c r="O81" s="2"/>
       <c r="P81" s="2"/>
     </row>
-    <row r="82" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -3334,7 +3349,7 @@
       <c r="O82" s="2"/>
       <c r="P82" s="2"/>
     </row>
-    <row r="83" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -3352,7 +3367,7 @@
       <c r="O83" s="2"/>
       <c r="P83" s="2"/>
     </row>
-    <row r="84" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -3370,7 +3385,7 @@
       <c r="O84" s="2"/>
       <c r="P84" s="2"/>
     </row>
-    <row r="85" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -3388,7 +3403,7 @@
       <c r="O85" s="2"/>
       <c r="P85" s="2"/>
     </row>
-    <row r="86" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -3406,7 +3421,7 @@
       <c r="O86" s="2"/>
       <c r="P86" s="2"/>
     </row>
-    <row r="87" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -3424,7 +3439,7 @@
       <c r="O87" s="2"/>
       <c r="P87" s="2"/>
     </row>
-    <row r="88" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -3442,7 +3457,7 @@
       <c r="O88" s="2"/>
       <c r="P88" s="2"/>
     </row>
-    <row r="89" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -3460,7 +3475,7 @@
       <c r="O89" s="2"/>
       <c r="P89" s="2"/>
     </row>
-    <row r="90" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -3478,7 +3493,7 @@
       <c r="O90" s="2"/>
       <c r="P90" s="2"/>
     </row>
-    <row r="91" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -3496,7 +3511,7 @@
       <c r="O91" s="2"/>
       <c r="P91" s="2"/>
     </row>
-    <row r="92" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -3514,7 +3529,7 @@
       <c r="O92" s="2"/>
       <c r="P92" s="2"/>
     </row>
-    <row r="93" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -3532,7 +3547,7 @@
       <c r="O93" s="2"/>
       <c r="P93" s="2"/>
     </row>
-    <row r="94" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -3550,7 +3565,7 @@
       <c r="O94" s="2"/>
       <c r="P94" s="2"/>
     </row>
-    <row r="95" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -3568,7 +3583,7 @@
       <c r="O95" s="2"/>
       <c r="P95" s="2"/>
     </row>
-    <row r="96" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -3586,7 +3601,7 @@
       <c r="O96" s="2"/>
       <c r="P96" s="2"/>
     </row>
-    <row r="97" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -3604,7 +3619,7 @@
       <c r="O97" s="2"/>
       <c r="P97" s="2"/>
     </row>
-    <row r="98" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -3622,7 +3637,7 @@
       <c r="O98" s="2"/>
       <c r="P98" s="2"/>
     </row>
-    <row r="99" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -3640,7 +3655,7 @@
       <c r="O99" s="2"/>
       <c r="P99" s="2"/>
     </row>
-    <row r="100" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -3658,7 +3673,7 @@
       <c r="O100" s="2"/>
       <c r="P100" s="2"/>
     </row>
-    <row r="101" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -3676,7 +3691,7 @@
       <c r="O101" s="2"/>
       <c r="P101" s="2"/>
     </row>
-    <row r="102" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -3694,7 +3709,7 @@
       <c r="O102" s="2"/>
       <c r="P102" s="2"/>
     </row>
-    <row r="103" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -3712,7 +3727,7 @@
       <c r="O103" s="2"/>
       <c r="P103" s="2"/>
     </row>
-    <row r="104" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -3730,7 +3745,7 @@
       <c r="O104" s="2"/>
       <c r="P104" s="2"/>
     </row>
-    <row r="105" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -3748,7 +3763,7 @@
       <c r="O105" s="2"/>
       <c r="P105" s="2"/>
     </row>
-    <row r="106" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3766,7 +3781,7 @@
       <c r="O106" s="2"/>
       <c r="P106" s="2"/>
     </row>
-    <row r="107" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -3784,7 +3799,7 @@
       <c r="O107" s="2"/>
       <c r="P107" s="2"/>
     </row>
-    <row r="108" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -3802,7 +3817,7 @@
       <c r="O108" s="2"/>
       <c r="P108" s="2"/>
     </row>
-    <row r="109" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -3820,7 +3835,7 @@
       <c r="O109" s="2"/>
       <c r="P109" s="2"/>
     </row>
-    <row r="110" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -3838,7 +3853,7 @@
       <c r="O110" s="2"/>
       <c r="P110" s="2"/>
     </row>
-    <row r="111" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -3856,7 +3871,7 @@
       <c r="O111" s="2"/>
       <c r="P111" s="2"/>
     </row>
-    <row r="112" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -3874,7 +3889,7 @@
       <c r="O112" s="2"/>
       <c r="P112" s="2"/>
     </row>
-    <row r="113" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -3892,7 +3907,7 @@
       <c r="O113" s="2"/>
       <c r="P113" s="2"/>
     </row>
-    <row r="114" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -3910,7 +3925,7 @@
       <c r="O114" s="2"/>
       <c r="P114" s="2"/>
     </row>
-    <row r="115" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -3928,7 +3943,7 @@
       <c r="O115" s="2"/>
       <c r="P115" s="2"/>
     </row>
-    <row r="116" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -3946,7 +3961,7 @@
       <c r="O116" s="2"/>
       <c r="P116" s="2"/>
     </row>
-    <row r="117" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -3964,7 +3979,7 @@
       <c r="O117" s="2"/>
       <c r="P117" s="2"/>
     </row>
-    <row r="118" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -3982,7 +3997,7 @@
       <c r="O118" s="2"/>
       <c r="P118" s="2"/>
     </row>
-    <row r="119" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -4000,7 +4015,7 @@
       <c r="O119" s="2"/>
       <c r="P119" s="2"/>
     </row>
-    <row r="120" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -4018,7 +4033,7 @@
       <c r="O120" s="2"/>
       <c r="P120" s="2"/>
     </row>
-    <row r="121" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -4036,7 +4051,7 @@
       <c r="O121" s="2"/>
       <c r="P121" s="2"/>
     </row>
-    <row r="122" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -4054,7 +4069,7 @@
       <c r="O122" s="2"/>
       <c r="P122" s="2"/>
     </row>
-    <row r="123" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -4072,7 +4087,7 @@
       <c r="O123" s="2"/>
       <c r="P123" s="2"/>
     </row>
-    <row r="124" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -4090,7 +4105,7 @@
       <c r="O124" s="2"/>
       <c r="P124" s="2"/>
     </row>
-    <row r="125" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -4108,7 +4123,7 @@
       <c r="O125" s="2"/>
       <c r="P125" s="2"/>
     </row>
-    <row r="126" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -4126,7 +4141,7 @@
       <c r="O126" s="2"/>
       <c r="P126" s="2"/>
     </row>
-    <row r="127" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -4144,7 +4159,7 @@
       <c r="O127" s="2"/>
       <c r="P127" s="2"/>
     </row>
-    <row r="128" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -4162,7 +4177,7 @@
       <c r="O128" s="2"/>
       <c r="P128" s="2"/>
     </row>
-    <row r="129" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -4180,7 +4195,7 @@
       <c r="O129" s="2"/>
       <c r="P129" s="2"/>
     </row>
-    <row r="130" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -4198,7 +4213,7 @@
       <c r="O130" s="2"/>
       <c r="P130" s="2"/>
     </row>
-    <row r="131" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -4216,7 +4231,7 @@
       <c r="O131" s="2"/>
       <c r="P131" s="2"/>
     </row>
-    <row r="132" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -4234,7 +4249,7 @@
       <c r="O132" s="2"/>
       <c r="P132" s="2"/>
     </row>
-    <row r="133" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>
@@ -4252,7 +4267,7 @@
       <c r="O133" s="2"/>
       <c r="P133" s="2"/>
     </row>
-    <row r="134" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="2"/>
       <c r="C134" s="2"/>
@@ -4270,7 +4285,7 @@
       <c r="O134" s="2"/>
       <c r="P134" s="2"/>
     </row>
-    <row r="135" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
       <c r="B135" s="2"/>
       <c r="C135" s="2"/>
@@ -4288,7 +4303,7 @@
       <c r="O135" s="2"/>
       <c r="P135" s="2"/>
     </row>
-    <row r="136" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
       <c r="B136" s="2"/>
       <c r="C136" s="2"/>
@@ -4306,7 +4321,7 @@
       <c r="O136" s="2"/>
       <c r="P136" s="2"/>
     </row>
-    <row r="137" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2"/>
@@ -4324,7 +4339,7 @@
       <c r="O137" s="2"/>
       <c r="P137" s="2"/>
     </row>
-    <row r="138" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
       <c r="B138" s="2"/>
       <c r="C138" s="2"/>
@@ -4342,7 +4357,7 @@
       <c r="O138" s="2"/>
       <c r="P138" s="2"/>
     </row>
-    <row r="139" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
       <c r="B139" s="2"/>
       <c r="C139" s="2"/>
@@ -4360,7 +4375,7 @@
       <c r="O139" s="2"/>
       <c r="P139" s="2"/>
     </row>
-    <row r="140" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
       <c r="B140" s="2"/>
       <c r="C140" s="2"/>
@@ -4378,7 +4393,7 @@
       <c r="O140" s="2"/>
       <c r="P140" s="2"/>
     </row>
-    <row r="141" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
       <c r="B141" s="2"/>
       <c r="C141" s="2"/>
@@ -4396,7 +4411,7 @@
       <c r="O141" s="2"/>
       <c r="P141" s="2"/>
     </row>
-    <row r="142" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
       <c r="B142" s="2"/>
       <c r="C142" s="2"/>
@@ -4414,7 +4429,7 @@
       <c r="O142" s="2"/>
       <c r="P142" s="2"/>
     </row>
-    <row r="143" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
       <c r="B143" s="2"/>
       <c r="C143" s="2"/>
@@ -4432,7 +4447,7 @@
       <c r="O143" s="2"/>
       <c r="P143" s="2"/>
     </row>
-    <row r="144" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
       <c r="B144" s="2"/>
       <c r="C144" s="2"/>
@@ -4450,7 +4465,7 @@
       <c r="O144" s="2"/>
       <c r="P144" s="2"/>
     </row>
-    <row r="145" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
       <c r="B145" s="2"/>
       <c r="C145" s="2"/>
@@ -4468,7 +4483,7 @@
       <c r="O145" s="2"/>
       <c r="P145" s="2"/>
     </row>
-    <row r="146" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
       <c r="B146" s="2"/>
       <c r="C146" s="2"/>
@@ -4486,7 +4501,7 @@
       <c r="O146" s="2"/>
       <c r="P146" s="2"/>
     </row>
-    <row r="147" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
       <c r="B147" s="2"/>
       <c r="C147" s="2"/>
@@ -4504,7 +4519,7 @@
       <c r="O147" s="2"/>
       <c r="P147" s="2"/>
     </row>
-    <row r="148" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
@@ -4522,7 +4537,7 @@
       <c r="O148" s="2"/>
       <c r="P148" s="2"/>
     </row>
-    <row r="149" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
@@ -4540,7 +4555,7 @@
       <c r="O149" s="2"/>
       <c r="P149" s="2"/>
     </row>
-    <row r="150" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
@@ -4558,7 +4573,7 @@
       <c r="O150" s="2"/>
       <c r="P150" s="2"/>
     </row>
-    <row r="151" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
@@ -4576,7 +4591,7 @@
       <c r="O151" s="2"/>
       <c r="P151" s="2"/>
     </row>
-    <row r="152" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -4594,7 +4609,7 @@
       <c r="O152" s="2"/>
       <c r="P152" s="2"/>
     </row>
-    <row r="153" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" s="2"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -4612,7 +4627,7 @@
       <c r="O153" s="2"/>
       <c r="P153" s="2"/>
     </row>
-    <row r="154" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" s="2"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -4630,7 +4645,7 @@
       <c r="O154" s="2"/>
       <c r="P154" s="2"/>
     </row>
-    <row r="155" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" s="2"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -4648,7 +4663,7 @@
       <c r="O155" s="2"/>
       <c r="P155" s="2"/>
     </row>
-    <row r="156" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -4666,7 +4681,7 @@
       <c r="O156" s="2"/>
       <c r="P156" s="2"/>
     </row>
-    <row r="157" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" s="2"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -4684,7 +4699,7 @@
       <c r="O157" s="2"/>
       <c r="P157" s="2"/>
     </row>
-    <row r="158" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -4702,7 +4717,7 @@
       <c r="O158" s="2"/>
       <c r="P158" s="2"/>
     </row>
-    <row r="159" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" s="2"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -4720,7 +4735,7 @@
       <c r="O159" s="2"/>
       <c r="P159" s="2"/>
     </row>
-    <row r="160" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" s="2"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -4738,7 +4753,7 @@
       <c r="O160" s="2"/>
       <c r="P160" s="2"/>
     </row>
-    <row r="161" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" s="2"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -4756,7 +4771,7 @@
       <c r="O161" s="2"/>
       <c r="P161" s="2"/>
     </row>
-    <row r="162" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162" s="2"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -4774,7 +4789,7 @@
       <c r="O162" s="2"/>
       <c r="P162" s="2"/>
     </row>
-    <row r="163" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" s="2"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -4792,7 +4807,7 @@
       <c r="O163" s="2"/>
       <c r="P163" s="2"/>
     </row>
-    <row r="164" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" s="2"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -4810,7 +4825,7 @@
       <c r="O164" s="2"/>
       <c r="P164" s="2"/>
     </row>
-    <row r="165" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" s="2"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -4828,7 +4843,7 @@
       <c r="O165" s="2"/>
       <c r="P165" s="2"/>
     </row>
-    <row r="166" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" s="2"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -4846,7 +4861,7 @@
       <c r="O166" s="2"/>
       <c r="P166" s="2"/>
     </row>
-    <row r="167" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" s="2"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -4864,7 +4879,7 @@
       <c r="O167" s="2"/>
       <c r="P167" s="2"/>
     </row>
-    <row r="168" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168" s="2"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -4882,7 +4897,7 @@
       <c r="O168" s="2"/>
       <c r="P168" s="2"/>
     </row>
-    <row r="169" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" s="2"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -4900,7 +4915,7 @@
       <c r="O169" s="2"/>
       <c r="P169" s="2"/>
     </row>
-    <row r="170" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" s="2"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -4918,7 +4933,7 @@
       <c r="O170" s="2"/>
       <c r="P170" s="2"/>
     </row>
-    <row r="171" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -4936,7 +4951,7 @@
       <c r="O171" s="2"/>
       <c r="P171" s="2"/>
     </row>
-    <row r="172" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -4954,7 +4969,7 @@
       <c r="O172" s="2"/>
       <c r="P172" s="2"/>
     </row>
-    <row r="173" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -4972,7 +4987,7 @@
       <c r="O173" s="2"/>
       <c r="P173" s="2"/>
     </row>
-    <row r="174" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -4990,7 +5005,7 @@
       <c r="O174" s="2"/>
       <c r="P174" s="2"/>
     </row>
-    <row r="175" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -5008,7 +5023,7 @@
       <c r="O175" s="2"/>
       <c r="P175" s="2"/>
     </row>
-    <row r="176" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -5026,7 +5041,7 @@
       <c r="O176" s="2"/>
       <c r="P176" s="2"/>
     </row>
-    <row r="177" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -5044,7 +5059,7 @@
       <c r="O177" s="2"/>
       <c r="P177" s="2"/>
     </row>
-    <row r="178" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -5062,7 +5077,7 @@
       <c r="O178" s="2"/>
       <c r="P178" s="2"/>
     </row>
-    <row r="179" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -5080,7 +5095,7 @@
       <c r="O179" s="2"/>
       <c r="P179" s="2"/>
     </row>
-    <row r="180" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -5098,7 +5113,7 @@
       <c r="O180" s="2"/>
       <c r="P180" s="2"/>
     </row>
-    <row r="181" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -5116,7 +5131,7 @@
       <c r="O181" s="2"/>
       <c r="P181" s="2"/>
     </row>
-    <row r="182" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -5134,7 +5149,7 @@
       <c r="O182" s="2"/>
       <c r="P182" s="2"/>
     </row>
-    <row r="183" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -5152,7 +5167,7 @@
       <c r="O183" s="2"/>
       <c r="P183" s="2"/>
     </row>
-    <row r="184" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -5170,7 +5185,7 @@
       <c r="O184" s="2"/>
       <c r="P184" s="2"/>
     </row>
-    <row r="185" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
@@ -5188,7 +5203,7 @@
       <c r="O185" s="2"/>
       <c r="P185" s="2"/>
     </row>
-    <row r="186" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
@@ -5206,7 +5221,7 @@
       <c r="O186" s="2"/>
       <c r="P186" s="2"/>
     </row>
-    <row r="187" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
@@ -5224,7 +5239,7 @@
       <c r="O187" s="2"/>
       <c r="P187" s="2"/>
     </row>
-    <row r="188" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
@@ -5242,7 +5257,7 @@
       <c r="O188" s="2"/>
       <c r="P188" s="2"/>
     </row>
-    <row r="189" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
@@ -5260,7 +5275,7 @@
       <c r="O189" s="2"/>
       <c r="P189" s="2"/>
     </row>
-    <row r="190" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
@@ -5278,7 +5293,7 @@
       <c r="O190" s="2"/>
       <c r="P190" s="2"/>
     </row>
-    <row r="191" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
@@ -5296,7 +5311,7 @@
       <c r="O191" s="2"/>
       <c r="P191" s="2"/>
     </row>
-    <row r="192" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
@@ -5314,7 +5329,7 @@
       <c r="O192" s="2"/>
       <c r="P192" s="2"/>
     </row>
-    <row r="193" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
@@ -5332,7 +5347,7 @@
       <c r="O193" s="2"/>
       <c r="P193" s="2"/>
     </row>
-    <row r="194" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
@@ -5350,7 +5365,7 @@
       <c r="O194" s="2"/>
       <c r="P194" s="2"/>
     </row>
-    <row r="195" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
@@ -5368,7 +5383,7 @@
       <c r="O195" s="2"/>
       <c r="P195" s="2"/>
     </row>
-    <row r="196" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
@@ -5386,7 +5401,7 @@
       <c r="O196" s="2"/>
       <c r="P196" s="2"/>
     </row>
-    <row r="197" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
@@ -5404,7 +5419,7 @@
       <c r="O197" s="2"/>
       <c r="P197" s="2"/>
     </row>
-    <row r="198" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
@@ -5422,7 +5437,7 @@
       <c r="O198" s="2"/>
       <c r="P198" s="2"/>
     </row>
-    <row r="199" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
@@ -5440,7 +5455,7 @@
       <c r="O199" s="2"/>
       <c r="P199" s="2"/>
     </row>
-    <row r="200" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
       <c r="C200" s="2"/>
@@ -5458,7 +5473,7 @@
       <c r="O200" s="2"/>
       <c r="P200" s="2"/>
     </row>
-    <row r="201" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
       <c r="C201" s="2"/>
@@ -5476,7 +5491,7 @@
       <c r="O201" s="2"/>
       <c r="P201" s="2"/>
     </row>
-    <row r="202" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
@@ -5494,7 +5509,7 @@
       <c r="O202" s="2"/>
       <c r="P202" s="2"/>
     </row>
-    <row r="203" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
@@ -5512,7 +5527,7 @@
       <c r="O203" s="2"/>
       <c r="P203" s="2"/>
     </row>
-    <row r="204" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
@@ -5530,7 +5545,7 @@
       <c r="O204" s="2"/>
       <c r="P204" s="2"/>
     </row>
-    <row r="205" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
@@ -5548,7 +5563,7 @@
       <c r="O205" s="2"/>
       <c r="P205" s="2"/>
     </row>
-    <row r="206" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
@@ -5566,7 +5581,7 @@
       <c r="O206" s="2"/>
       <c r="P206" s="2"/>
     </row>
-    <row r="207" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
@@ -5584,7 +5599,7 @@
       <c r="O207" s="2"/>
       <c r="P207" s="2"/>
     </row>
-    <row r="208" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
@@ -5602,7 +5617,7 @@
       <c r="O208" s="2"/>
       <c r="P208" s="2"/>
     </row>
-    <row r="209" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
@@ -5620,115 +5635,115 @@
       <c r="O209" s="2"/>
       <c r="P209" s="2"/>
     </row>
-    <row r="210" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
       <c r="D210" s="2"/>
     </row>
-    <row r="211" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
       <c r="D211" s="2"/>
     </row>
-    <row r="212" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
       <c r="D212" s="2"/>
     </row>
-    <row r="213" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
       <c r="D213" s="2"/>
     </row>
-    <row r="214" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
       <c r="D214" s="2"/>
     </row>
-    <row r="215" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
       <c r="D215" s="2"/>
     </row>
-    <row r="216" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="2"/>
     </row>
-    <row r="217" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
       <c r="D217" s="2"/>
     </row>
-    <row r="218" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
       <c r="D218" s="2"/>
     </row>
-    <row r="219" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
       <c r="D219" s="2"/>
     </row>
-    <row r="220" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
       <c r="D220" s="2"/>
     </row>
-    <row r="221" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
       <c r="D221" s="2"/>
     </row>
-    <row r="222" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
       <c r="D222" s="2"/>
     </row>
-    <row r="223" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
       <c r="D223" s="2"/>
     </row>
-    <row r="224" spans="1:16" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
       <c r="D224" s="2"/>
     </row>
-    <row r="225" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
       <c r="D225" s="2"/>
     </row>
-    <row r="226" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
       <c r="D226" s="2"/>
     </row>
-    <row r="227" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
       <c r="D227" s="2"/>
     </row>
-    <row r="228" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
@@ -5742,11 +5757,11 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" display="https://github.com/Chen-Qixian"/>
-    <hyperlink ref="C6" r:id="rId2" display="https://github.com/L-Richard"/>
-    <hyperlink ref="F6" r:id="rId3" display="https://github.com/Soengseon972"/>
-    <hyperlink ref="E6" r:id="rId4" display="https://github.com/sqbuaa"/>
-    <hyperlink ref="D6" r:id="rId5" display="https://github.com/EurusQF"/>
+    <hyperlink ref="B6" r:id="rId1" display="https://github.com/Chen-Qixian" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C6" r:id="rId2" display="https://github.com/L-Richard" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F6" r:id="rId3" display="https://github.com/Soengseon972" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E6" r:id="rId4" display="https://github.com/sqbuaa" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D6" r:id="rId5" display="https://github.com/EurusQF" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
@@ -5754,22 +5769,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.08203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" ht="21.5" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>17</v>
       </c>
@@ -5777,7 +5792,7 @@
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
     </row>
-    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
@@ -5791,7 +5806,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -5805,7 +5820,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -5819,7 +5834,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -5833,7 +5848,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -5847,7 +5862,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -5861,7 +5876,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -5875,7 +5890,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -5889,7 +5904,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -5903,7 +5918,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -5917,7 +5932,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -5931,7 +5946,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -5945,7 +5960,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -5959,7 +5974,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -5973,7 +5988,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -5987,7 +6002,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -6001,7 +6016,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -6015,7 +6030,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>17</v>
       </c>
@@ -6029,7 +6044,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -6043,7 +6058,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>19</v>
       </c>
@@ -6067,24 +6082,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.75" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="61.375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="61.33203125" style="9" customWidth="1"/>
     <col min="4" max="4" width="29.25" style="9" customWidth="1"/>
-    <col min="5" max="5" width="13.625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="13.58203125" style="9" customWidth="1"/>
     <col min="6" max="16384" width="9" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="21.5" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>13</v>
       </c>
@@ -6093,7 +6108,7 @@
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
@@ -6110,7 +6125,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -6127,7 +6142,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -6144,7 +6159,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -6161,7 +6176,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -6172,13 +6187,13 @@
         <v>43</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -6189,13 +6204,13 @@
         <v>44</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E7" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -6206,13 +6221,13 @@
         <v>46</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -6223,13 +6238,13 @@
         <v>50</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E9" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -6240,13 +6255,13 @@
         <v>48</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -6257,13 +6272,13 @@
         <v>53</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E11" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>10</v>
       </c>
@@ -6280,7 +6295,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -6291,13 +6306,13 @@
         <v>55</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -6308,13 +6323,13 @@
         <v>57</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -6331,7 +6346,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -6348,7 +6363,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -6365,7 +6380,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -6382,7 +6397,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>17</v>
       </c>
@@ -6399,7 +6414,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -6416,7 +6431,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>19</v>
       </c>
@@ -6433,7 +6448,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>20</v>
       </c>
@@ -6450,7 +6465,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>21</v>
       </c>
@@ -6467,7 +6482,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>22</v>
       </c>
@@ -6484,7 +6499,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>23</v>
       </c>
@@ -6501,7 +6516,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>24</v>
       </c>
@@ -6518,7 +6533,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>25</v>
       </c>
@@ -6535,7 +6550,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>26</v>
       </c>
@@ -6552,7 +6567,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>27</v>
       </c>
@@ -6569,259 +6584,293 @@
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>28</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>156</v>
+        <v>278</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>157</v>
+        <v>279</v>
       </c>
       <c r="D30" s="26">
-        <v>234</v>
+        <v>33</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>29</v>
       </c>
-      <c r="B31" s="10">
-        <v>4662817</v>
+      <c r="B31" s="10" t="s">
+        <v>156</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>228</v>
+        <v>157</v>
       </c>
       <c r="D31" s="26">
-        <v>659</v>
+        <v>234</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>30</v>
       </c>
-      <c r="B32" s="10">
-        <v>1707673</v>
+      <c r="B32" s="10" t="s">
+        <v>276</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>229</v>
+        <v>277</v>
       </c>
       <c r="D32" s="26">
-        <v>113</v>
+        <v>248</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>31</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>230</v>
+      <c r="B33" s="10">
+        <v>4662817</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D33" s="26">
-        <v>72</v>
+        <v>659</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>32</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>232</v>
+      <c r="B34" s="10">
+        <v>1707673</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D34" s="26">
-        <v>12811</v>
+        <v>113</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="10">
         <v>33</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D35" s="26">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <v>34</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D36" s="26">
-        <v>81</v>
+        <v>12811</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="10">
         <v>35</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C37" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="D37" s="26">
+        <v>93</v>
+      </c>
+      <c r="E37" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="D37" s="26">
-        <v>0</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="10">
         <v>36</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="D38" s="26">
         <v>81</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <v>37</v>
       </c>
-      <c r="B39" s="30" t="s">
-        <v>242</v>
+      <c r="B39" s="10" t="s">
+        <v>236</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="D39" s="26">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="10">
         <v>38</v>
       </c>
-      <c r="B40" s="30" t="s">
-        <v>244</v>
+      <c r="B40" s="10" t="s">
+        <v>239</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D40" s="26">
-        <v>2677</v>
+        <v>81</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="10">
         <v>39</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D41" s="26">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="10">
         <v>40</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="D42" s="26">
-        <v>77524</v>
+        <v>2677</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="10">
         <v>41</v>
       </c>
       <c r="B43" s="30" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D43" s="26">
-        <v>177</v>
+        <v>0</v>
       </c>
       <c r="E43" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="10">
         <v>42</v>
       </c>
       <c r="B44" s="30" t="s">
+        <v>247</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D44" s="26">
+        <v>77524</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="C44" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="D44" s="26">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="10">
+        <v>43</v>
+      </c>
+      <c r="B45" s="30" t="s">
+        <v>248</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="D45" s="26">
+        <v>177</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="10">
+        <v>44</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="D46" s="26">
         <v>56</v>
       </c>
-      <c r="E44" s="10" t="s">
-        <v>252</v>
+      <c r="E46" s="10" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -6835,23 +6884,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.58203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.75" customWidth="1"/>
     <col min="5" max="5" width="40.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" ht="21.5" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>14</v>
       </c>
@@ -6860,7 +6909,7 @@
       <c r="D1" s="38"/>
       <c r="E1" s="38"/>
     </row>
-    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
@@ -6877,7 +6926,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="34.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" ht="33" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>1</v>
       </c>
@@ -6894,7 +6943,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="51.75" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>2</v>
       </c>
@@ -6911,7 +6960,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="34.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="33" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>3</v>
       </c>
@@ -6926,331 +6975,331 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="34.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="33" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>4</v>
       </c>
       <c r="B6" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>168</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>169</v>
       </c>
       <c r="D6" s="23"/>
       <c r="E6" s="24" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>5</v>
       </c>
       <c r="B7" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="D7" s="23" t="s">
         <v>172</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="E7" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="E7" s="24" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>6</v>
       </c>
       <c r="B8" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="D8" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>177</v>
-      </c>
       <c r="E8" s="24" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>7</v>
       </c>
       <c r="B9" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" s="22" t="s">
         <v>178</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>179</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="24" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>8</v>
       </c>
       <c r="B10" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" s="22" t="s">
         <v>181</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>182</v>
       </c>
       <c r="D10" s="23"/>
       <c r="E10" s="24" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>9</v>
       </c>
       <c r="B11" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" s="22" t="s">
         <v>183</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>184</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="24" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>10</v>
       </c>
       <c r="B12" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C12" s="22" t="s">
         <v>185</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>186</v>
       </c>
       <c r="D12" s="23"/>
       <c r="E12" s="24" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>11</v>
       </c>
       <c r="B13" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13" s="22" t="s">
         <v>188</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>189</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="24" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="34.5" x14ac:dyDescent="0.15">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="33" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>12</v>
       </c>
       <c r="B14" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="C14" s="22" t="s">
         <v>191</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>192</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="24" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <v>13</v>
       </c>
       <c r="B15" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>193</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>194</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="24" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>14</v>
       </c>
       <c r="B16" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>196</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>197</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="24" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>15</v>
       </c>
       <c r="B17" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>198</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>199</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="24" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <v>16</v>
       </c>
       <c r="B18" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="C18" s="22" t="s">
         <v>200</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>201</v>
       </c>
       <c r="D18" s="25"/>
       <c r="E18" s="24" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="42.75" x14ac:dyDescent="0.15">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
         <v>17</v>
       </c>
       <c r="B19" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="C19" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="D19" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="D19" s="23" t="s">
+      <c r="E19" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="E19" s="23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <v>18</v>
       </c>
       <c r="B20" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="C20" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="D20" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>208</v>
-      </c>
       <c r="E20" s="23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="21">
         <v>19</v>
       </c>
       <c r="B21" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="C21" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="D21" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="D21" s="23" t="s">
-        <v>211</v>
-      </c>
       <c r="E21" s="23" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="28.5" x14ac:dyDescent="0.15">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="21">
         <v>20</v>
       </c>
       <c r="B22" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="C22" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="D22" s="23" t="s">
         <v>213</v>
       </c>
-      <c r="D22" s="23" t="s">
+      <c r="E22" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="E22" s="23" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+    </row>
+    <row r="23" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="21">
         <v>21</v>
       </c>
       <c r="B23" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>216</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>217</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="23" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <v>22</v>
       </c>
       <c r="B24" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="C24" s="22" t="s">
         <v>219</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>220</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="23" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="21">
         <v>23</v>
       </c>
       <c r="B25" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C25" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>223</v>
       </c>
       <c r="D25" s="23"/>
       <c r="E25" s="23" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="17.25" x14ac:dyDescent="0.15">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="21">
         <v>24</v>
       </c>
       <c r="B26" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="C26" s="22" t="s">
         <v>225</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>226</v>
       </c>
       <c r="D26" s="23"/>
       <c r="E26" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>